<commit_message>
added edit column types button
</commit_message>
<xml_diff>
--- a/data/toy_animal_trial_repeated.xlsx
+++ b/data/toy_animal_trial_repeated.xlsx
@@ -392,7 +392,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>48.50972295728553</v>
+        <v>45.14471178787333</v>
       </c>
     </row>
     <row r="3">
@@ -408,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>53.67039420099835</v>
+        <v>51.02560677949042</v>
       </c>
     </row>
     <row r="4">
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>56.47908264602592</v>
+        <v>53.77052470619385</v>
       </c>
     </row>
     <row r="5">
@@ -440,7 +440,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>63.21894406190453</v>
+        <v>61.75700659403199</v>
       </c>
     </row>
     <row r="6">
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>63.62894150748009</v>
+        <v>61.3036698547994</v>
       </c>
     </row>
     <row r="7">
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>67.63900424887984</v>
+        <v>65.65042017666575</v>
       </c>
     </row>
     <row r="8">
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>52.45400475498733</v>
+        <v>51.50474804170551</v>
       </c>
     </row>
     <row r="9">
@@ -504,7 +504,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>55.41103364915949</v>
+        <v>54.44745323393506</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>62.64545187307681</v>
+        <v>63.09334419915815</v>
       </c>
     </row>
     <row r="11">
@@ -536,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>60.86233206405564</v>
+        <v>59.71585112046326</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>69.08905683432205</v>
+        <v>69.68481748081848</v>
       </c>
     </row>
     <row r="13">
@@ -568,7 +568,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>62.89338660834277</v>
+        <v>60.42392384617944</v>
       </c>
     </row>
     <row r="14">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>57.87125787720646</v>
+        <v>64.69070488343903</v>
       </c>
     </row>
     <row r="15">
@@ -600,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>59.48897935983209</v>
+        <v>65.84766686027321</v>
       </c>
     </row>
     <row r="16">
@@ -616,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>62.76524133453017</v>
+        <v>69.21601615987063</v>
       </c>
     </row>
     <row r="17">
@@ -632,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>66.25633507657788</v>
+        <v>72.87080781593427</v>
       </c>
     </row>
     <row r="18">
@@ -648,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>66.61044626897034</v>
+        <v>72.34295607245754</v>
       </c>
     </row>
     <row r="19">
@@ -664,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="D19">
-        <v>70.11779447728999</v>
+        <v>76.01942035021706</v>
       </c>
     </row>
     <row r="20">
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>50.08529063352788</v>
+        <v>49.3487488161191</v>
       </c>
     </row>
     <row r="21">
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>52.92564310342242</v>
+        <v>52.13588544264515</v>
       </c>
     </row>
     <row r="22">
@@ -712,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>60.05160270706192</v>
+        <v>60.63716491416449</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>63.48564611873743</v>
+        <v>64.21588946306517</v>
       </c>
     </row>
     <row r="24">
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>65.30002946304066</v>
+        <v>65.63506725546948</v>
       </c>
     </row>
     <row r="25">
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="D25">
-        <v>70.90781918648837</v>
+        <v>72.11212022006642</v>
       </c>
     </row>
     <row r="26">
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>59.40882952720332</v>
+        <v>61.97606515347425</v>
       </c>
     </row>
     <row r="27">
@@ -792,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>54.78548197215229</v>
+        <v>54.81160174673953</v>
       </c>
     </row>
     <row r="28">
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="D28">
-        <v>52.33106884339946</v>
+        <v>50.53905090840242</v>
       </c>
     </row>
     <row r="29">
@@ -824,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>65.27579104370867</v>
+        <v>66.7986805088147</v>
       </c>
     </row>
     <row r="30">
@@ -840,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="D30">
-        <v>63.13097318257471</v>
+        <v>62.9389233606361</v>
       </c>
     </row>
     <row r="31">
@@ -856,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="D31">
-        <v>66.19454962091982</v>
+        <v>66.02369194509625</v>
       </c>
     </row>
     <row r="32">
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>59.50684408285666</v>
+        <v>67.39267540008649</v>
       </c>
     </row>
     <row r="33">
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>58.57581095261354</v>
+        <v>65.15129789309566</v>
       </c>
     </row>
     <row r="34">
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <v>58.76797683700295</v>
+        <v>64.40751907228154</v>
       </c>
     </row>
     <row r="35">
@@ -920,7 +920,7 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <v>65.97404041301402</v>
+        <v>73.01560384029629</v>
       </c>
     </row>
     <row r="36">
@@ -936,7 +936,7 @@
         <v>5</v>
       </c>
       <c r="D36">
-        <v>68.01345588644944</v>
+        <v>74.73482447154352</v>
       </c>
     </row>
     <row r="37">
@@ -952,7 +952,7 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <v>71.44742253146623</v>
+        <v>78.31344666489925</v>
       </c>
     </row>
     <row r="38">
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>55.0776736153574</v>
+        <v>57.30661884044054</v>
       </c>
     </row>
     <row r="39">
@@ -984,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>55.80985231660118</v>
+        <v>57.28285710876558</v>
       </c>
     </row>
     <row r="40">
@@ -1000,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <v>61.85496205753491</v>
+        <v>64.34300343001054</v>
       </c>
     </row>
     <row r="41">
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="D41">
-        <v>62.26037272652216</v>
+        <v>63.88355098866021</v>
       </c>
     </row>
     <row r="42">
@@ -1032,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="D42">
-        <v>66.91717830372549</v>
+        <v>69.09262509159799</v>
       </c>
     </row>
     <row r="43">
@@ -1048,7 +1048,7 @@
         <v>6</v>
       </c>
       <c r="D43">
-        <v>72.21234945142645</v>
+        <v>75.15285328853261</v>
       </c>
     </row>
     <row r="44">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>51.77542200328834</v>
+        <v>47.150358555696</v>
       </c>
     </row>
     <row r="45">
@@ -1080,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="D45">
-        <v>52.49208277419325</v>
+        <v>47.10590625023589</v>
       </c>
     </row>
     <row r="46">
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="D46">
-        <v>59.91630038614021</v>
+        <v>56.00486306616517</v>
       </c>
     </row>
     <row r="47">
@@ -1112,7 +1112,7 @@
         <v>4</v>
       </c>
       <c r="D47">
-        <v>62.45038909867329</v>
+        <v>58.38364801620927</v>
       </c>
     </row>
     <row r="48">
@@ -1128,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="D48">
-        <v>64.11506840931114</v>
+        <v>59.60322043039307</v>
       </c>
     </row>
     <row r="49">
@@ -1144,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="D49">
-        <v>66.18607273612126</v>
+        <v>61.36455953280656</v>
       </c>
     </row>
     <row r="50">
@@ -1160,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>49.74257606809483</v>
+        <v>46.36725858448136</v>
       </c>
     </row>
     <row r="51">
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="D51">
-        <v>58.70825164180297</v>
+        <v>57.32149268275887</v>
       </c>
     </row>
     <row r="52">
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <v>55.82551553477157</v>
+        <v>52.47784454005033</v>
       </c>
     </row>
     <row r="53">
@@ -1208,7 +1208,7 @@
         <v>4</v>
       </c>
       <c r="D53">
-        <v>67.18829327526268</v>
+        <v>66.62821486070516</v>
       </c>
     </row>
     <row r="54">
@@ -1224,7 +1224,7 @@
         <v>5</v>
       </c>
       <c r="D54">
-        <v>68.22412617476851</v>
+        <v>67.0093253933796</v>
       </c>
     </row>
     <row r="55">
@@ -1240,7 +1240,7 @@
         <v>6</v>
       </c>
       <c r="D55">
-        <v>65.91919321891152</v>
+        <v>62.93608145223693</v>
       </c>
     </row>
     <row r="56">
@@ -1256,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>49.02941335887974</v>
+        <v>46.22034457817313</v>
       </c>
     </row>
     <row r="57">
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="D57">
-        <v>52.97745636870218</v>
+        <v>50.48440192460305</v>
       </c>
     </row>
     <row r="58">
@@ -1288,7 +1288,7 @@
         <v>3</v>
       </c>
       <c r="D58">
-        <v>58.87932718726967</v>
+        <v>57.35356301602637</v>
       </c>
     </row>
     <row r="59">
@@ -1304,7 +1304,7 @@
         <v>4</v>
       </c>
       <c r="D59">
-        <v>60.36860042441296</v>
+        <v>58.33926066555076</v>
       </c>
     </row>
     <row r="60">
@@ -1320,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="D60">
-        <v>63.06604826160689</v>
+        <v>60.93585778180932</v>
       </c>
     </row>
     <row r="61">
@@ -1336,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="D61">
-        <v>64.25382035800504</v>
+        <v>61.51955391034019</v>
       </c>
     </row>
     <row r="62">
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>55.31308042045216</v>
+        <v>60.16437988540109</v>
       </c>
     </row>
     <row r="63">
@@ -1368,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>56.0934501865077</v>
+        <v>60.20487290680847</v>
       </c>
     </row>
     <row r="64">
@@ -1384,7 +1384,7 @@
         <v>3</v>
       </c>
       <c r="D64">
-        <v>56.44433778511451</v>
+        <v>59.67272303828423</v>
       </c>
     </row>
     <row r="65">
@@ -1400,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="D65">
-        <v>63.30748403401563</v>
+        <v>67.82358470348572</v>
       </c>
     </row>
     <row r="66">
@@ -1416,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="D66">
-        <v>70.20515342206122</v>
+        <v>76.02047722087984</v>
       </c>
     </row>
     <row r="67">
@@ -1432,7 +1432,7 @@
         <v>6</v>
       </c>
       <c r="D67">
-        <v>68.72212270705374</v>
+        <v>73.0431029342032</v>
       </c>
     </row>
     <row r="68">
@@ -1448,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>55.54352062078982</v>
+        <v>57.59074025124431</v>
       </c>
     </row>
     <row r="69">
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>51.86597952924723</v>
+        <v>51.68735212918752</v>
       </c>
     </row>
     <row r="70">
@@ -1480,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="D70">
-        <v>59.55294175754111</v>
+        <v>60.93663510024602</v>
       </c>
     </row>
     <row r="71">
@@ -1496,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="D71">
-        <v>64.27784926594511</v>
+        <v>66.23651177811803</v>
       </c>
     </row>
     <row r="72">
@@ -1512,7 +1512,7 @@
         <v>5</v>
       </c>
       <c r="D72">
-        <v>66.62308774061488</v>
+        <v>68.36349641101104</v>
       </c>
     </row>
     <row r="73">
@@ -1528,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="D73">
-        <v>69.03665623656156</v>
+        <v>70.58158773893996</v>
       </c>
     </row>
     <row r="74">
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>51.87942487627198</v>
+        <v>52.84180467034281</v>
       </c>
     </row>
     <row r="75">
@@ -1560,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>54.25242986308736</v>
+        <v>55.00581131942999</v>
       </c>
     </row>
     <row r="76">
@@ -1576,7 +1576,7 @@
         <v>3</v>
       </c>
       <c r="D76">
-        <v>56.72915652937337</v>
+        <v>57.30811354114466</v>
       </c>
     </row>
     <row r="77">
@@ -1592,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="D77">
-        <v>63.15448269248849</v>
+        <v>64.87521509196482</v>
       </c>
     </row>
     <row r="78">
@@ -1608,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="D78">
-        <v>62.9591190586337</v>
+        <v>63.6147302468251</v>
       </c>
     </row>
     <row r="79">
@@ -1624,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="D79">
-        <v>67.3298705700861</v>
+        <v>68.44239892876163</v>
       </c>
     </row>
     <row r="80">
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>52.4530888552955</v>
+        <v>52.63972752687773</v>
       </c>
     </row>
     <row r="81">
@@ -1656,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="D81">
-        <v>61.75295144758687</v>
+        <v>64.03954431659955</v>
       </c>
     </row>
     <row r="82">
@@ -1672,7 +1672,7 @@
         <v>3</v>
       </c>
       <c r="D82">
-        <v>57.26551572680387</v>
+        <v>57.05629668888889</v>
       </c>
     </row>
     <row r="83">
@@ -1688,7 +1688,7 @@
         <v>4</v>
       </c>
       <c r="D83">
-        <v>62.92752514874481</v>
+        <v>63.60564258481014</v>
       </c>
     </row>
     <row r="84">
@@ -1704,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="D84">
-        <v>65.45524798058136</v>
+        <v>65.97593969392555</v>
       </c>
     </row>
     <row r="85">
@@ -1720,7 +1720,7 @@
         <v>6</v>
       </c>
       <c r="D85">
-        <v>65.33579552949985</v>
+        <v>64.8166697591502</v>
       </c>
     </row>
     <row r="86">
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <v>51.67439347212105</v>
+        <v>49.37972084698115</v>
       </c>
     </row>
     <row r="87">
@@ -1752,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="D87">
-        <v>59.22197030576189</v>
+        <v>58.44315662516894</v>
       </c>
     </row>
     <row r="88">
@@ -1768,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="D88">
-        <v>59.24282988972949</v>
+        <v>57.4709694037924</v>
       </c>
     </row>
     <row r="89">
@@ -1784,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="D89">
-        <v>61.01201649647067</v>
+        <v>58.82988487944731</v>
       </c>
     </row>
     <row r="90">
@@ -1800,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="D90">
-        <v>62.62082723347297</v>
+        <v>59.97496586211705</v>
       </c>
     </row>
     <row r="91">
@@ -1816,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="D91">
-        <v>60.7285760658703</v>
+        <v>56.45196430531348</v>
       </c>
     </row>
     <row r="92">
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>62.76783791384868</v>
+        <v>71.04682767447517</v>
       </c>
     </row>
     <row r="93">
@@ -1848,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="D93">
-        <v>58.79190606083169</v>
+        <v>64.47891853711918</v>
       </c>
     </row>
     <row r="94">
@@ -1864,7 +1864,7 @@
         <v>3</v>
       </c>
       <c r="D94">
-        <v>69.19366880623815</v>
+        <v>77.08126886432781</v>
       </c>
     </row>
     <row r="95">
@@ -1880,7 +1880,7 @@
         <v>4</v>
       </c>
       <c r="D95">
-        <v>76.50113698125861</v>
+        <v>85.55789309768839</v>
       </c>
     </row>
     <row r="96">
@@ -1896,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="D96">
-        <v>70.24214679069075</v>
+        <v>75.94590617693127</v>
       </c>
     </row>
     <row r="97">
@@ -1912,7 +1912,7 @@
         <v>6</v>
       </c>
       <c r="D97">
-        <v>80.47917927973029</v>
+        <v>88.3286161623173</v>
       </c>
     </row>
     <row r="98">
@@ -1928,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <v>56.00910848825107</v>
+        <v>57.73831291176556</v>
       </c>
     </row>
     <row r="99">
@@ -1944,7 +1944,7 @@
         <v>2</v>
       </c>
       <c r="D99">
-        <v>55.87926847902202</v>
+        <v>56.29852623279348</v>
       </c>
     </row>
     <row r="100">
@@ -1960,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="D100">
-        <v>59.85169799511323</v>
+        <v>60.32843225424843</v>
       </c>
     </row>
     <row r="101">
@@ -1976,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="D101">
-        <v>63.3910924357347</v>
+        <v>63.78095817507706</v>
       </c>
     </row>
     <row r="102">
@@ -1992,7 +1992,7 @@
         <v>5</v>
       </c>
       <c r="D102">
-        <v>70.40298138994757</v>
+        <v>71.86347678069423</v>
       </c>
     </row>
     <row r="103">
@@ -2008,7 +2008,7 @@
         <v>6</v>
       </c>
       <c r="D103">
-        <v>71.41043420147078</v>
+        <v>71.94008052939184</v>
       </c>
     </row>
     <row r="104">
@@ -2024,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="D104">
-        <v>53.9305160056682</v>
+        <v>46.75196415212547</v>
       </c>
     </row>
     <row r="105">
@@ -2040,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="D105">
-        <v>61.96709250831774</v>
+        <v>56.20073282232486</v>
       </c>
     </row>
     <row r="106">
@@ -2056,7 +2056,7 @@
         <v>3</v>
       </c>
       <c r="D106">
-        <v>55.60567425863518</v>
+        <v>46.45217515608145</v>
       </c>
     </row>
     <row r="107">
@@ -2072,7 +2072,7 @@
         <v>4</v>
       </c>
       <c r="D107">
-        <v>65.62998222916626</v>
+        <v>58.55125245012288</v>
       </c>
     </row>
     <row r="108">
@@ -2088,7 +2088,7 @@
         <v>5</v>
       </c>
       <c r="D108">
-        <v>69.37389240974345</v>
+        <v>62.27646602422581</v>
       </c>
     </row>
     <row r="109">
@@ -2104,7 +2104,7 @@
         <v>6</v>
       </c>
       <c r="D109">
-        <v>71.86337342359107</v>
+        <v>64.32910737602263</v>
       </c>
     </row>
     <row r="110">
@@ -2120,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>54.17758197829635</v>
+        <v>55.97462897627408</v>
       </c>
     </row>
     <row r="111">
@@ -2136,7 +2136,7 @@
         <v>2</v>
       </c>
       <c r="D111">
-        <v>60.64435398323539</v>
+        <v>63.33032498285948</v>
       </c>
     </row>
     <row r="112">
@@ -2152,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="D112">
-        <v>63.96152579761662</v>
+        <v>66.48655406870112</v>
       </c>
     </row>
     <row r="113">
@@ -2168,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="D113">
-        <v>70.29168040278881</v>
+        <v>73.66009354226404</v>
       </c>
     </row>
     <row r="114">
@@ -2184,7 +2184,7 @@
         <v>5</v>
       </c>
       <c r="D114">
-        <v>71.28539553481589</v>
+        <v>73.71838038496679</v>
       </c>
     </row>
     <row r="115">
@@ -2200,7 +2200,7 @@
         <v>6</v>
       </c>
       <c r="D115">
-        <v>79.13363196318423</v>
+        <v>82.91602895612459</v>
       </c>
     </row>
     <row r="116">
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>53.73067461124309</v>
+        <v>51.46492812256433</v>
       </c>
     </row>
     <row r="117">
@@ -2232,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="D117">
-        <v>61.81255158128212</v>
+        <v>60.97409741594973</v>
       </c>
     </row>
     <row r="118">
@@ -2248,7 +2248,7 @@
         <v>3</v>
       </c>
       <c r="D118">
-        <v>59.30688616454593</v>
+        <v>56.36654352696814</v>
       </c>
     </row>
     <row r="119">
@@ -2264,7 +2264,7 @@
         <v>4</v>
       </c>
       <c r="D119">
-        <v>62.4739514502698</v>
+        <v>59.32263057459995</v>
       </c>
     </row>
     <row r="120">
@@ -2280,7 +2280,7 @@
         <v>5</v>
       </c>
       <c r="D120">
-        <v>79.77753698937136</v>
+        <v>81.12741129340201</v>
       </c>
     </row>
     <row r="121">
@@ -2296,7 +2296,7 @@
         <v>6</v>
       </c>
       <c r="D121">
-        <v>72.60384442006284</v>
+        <v>70.29582120099066</v>
       </c>
     </row>
     <row r="122">
@@ -2312,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="D122">
-        <v>54.55903536264845</v>
+        <v>50.58596813024179</v>
       </c>
     </row>
     <row r="123">
@@ -2328,7 +2328,7 @@
         <v>2</v>
       </c>
       <c r="D123">
-        <v>59.37406161012785</v>
+        <v>55.73933646021433</v>
       </c>
     </row>
     <row r="124">
@@ -2344,7 +2344,7 @@
         <v>3</v>
       </c>
       <c r="D124">
-        <v>59.81301071090007</v>
+        <v>55.05793526124395</v>
       </c>
     </row>
     <row r="125">
@@ -2360,7 +2360,7 @@
         <v>4</v>
       </c>
       <c r="D125">
-        <v>66.61493872096713</v>
+        <v>62.86050594133336</v>
       </c>
     </row>
     <row r="126">
@@ -2376,7 +2376,7 @@
         <v>5</v>
       </c>
       <c r="D126">
-        <v>69.97124617018156</v>
+        <v>66.06891587361928</v>
       </c>
     </row>
     <row r="127">
@@ -2392,7 +2392,7 @@
         <v>6</v>
       </c>
       <c r="D127">
-        <v>72.01821106510123</v>
+        <v>67.53153573351216</v>
       </c>
     </row>
     <row r="128">
@@ -2408,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="D128">
-        <v>55.55992927125935</v>
+        <v>54.75332264615149</v>
       </c>
     </row>
     <row r="129">
@@ -2424,7 +2424,7 @@
         <v>2</v>
       </c>
       <c r="D129">
-        <v>59.06184840946802</v>
+        <v>58.15588149709637</v>
       </c>
     </row>
     <row r="130">
@@ -2440,7 +2440,7 @@
         <v>3</v>
       </c>
       <c r="D130">
-        <v>69.34940586773195</v>
+        <v>70.60595810811495</v>
       </c>
     </row>
     <row r="131">
@@ -2456,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="D131">
-        <v>64.54004188186494</v>
+        <v>62.92680612695892</v>
       </c>
     </row>
     <row r="132">
@@ -2472,7 +2472,7 @@
         <v>5</v>
       </c>
       <c r="D132">
-        <v>67.27606136945943</v>
+        <v>65.30816544375158</v>
       </c>
     </row>
     <row r="133">
@@ -2488,7 +2488,7 @@
         <v>6</v>
       </c>
       <c r="D133">
-        <v>74.47741536819665</v>
+        <v>73.64330410873454</v>
       </c>
     </row>
     <row r="134">
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="D134">
-        <v>54.67943335171493</v>
+        <v>50.88589630792911</v>
       </c>
     </row>
     <row r="135">
@@ -2520,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="D135">
-        <v>58.85756154011607</v>
+        <v>55.1900672257973</v>
       </c>
     </row>
     <row r="136">
@@ -2536,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="D136">
-        <v>59.9728951052522</v>
+        <v>55.41051197931214</v>
       </c>
     </row>
     <row r="137">
@@ -2552,7 +2552,7 @@
         <v>4</v>
       </c>
       <c r="D137">
-        <v>61.95801270147195</v>
+        <v>56.7906687742718</v>
       </c>
     </row>
     <row r="138">
@@ -2568,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="D138">
-        <v>72.73754663165398</v>
+        <v>69.89671401451452</v>
       </c>
     </row>
     <row r="139">
@@ -2584,7 +2584,7 @@
         <v>6</v>
       </c>
       <c r="D139">
-        <v>71.69903993952485</v>
+        <v>67.24537175834233</v>
       </c>
     </row>
     <row r="140">
@@ -2600,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="D140">
-        <v>51.74567895345759</v>
+        <v>47.96460117363966</v>
       </c>
     </row>
     <row r="141">
@@ -2616,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="D141">
-        <v>57.43337883459444</v>
+        <v>54.28153434848878</v>
       </c>
     </row>
     <row r="142">
@@ -2632,7 +2632,7 @@
         <v>3</v>
       </c>
       <c r="D142">
-        <v>61.35068985837206</v>
+        <v>58.23794904685895</v>
       </c>
     </row>
     <row r="143">
@@ -2648,7 +2648,7 @@
         <v>4</v>
       </c>
       <c r="D143">
-        <v>69.07197841055864</v>
+        <v>67.26633378310773</v>
       </c>
     </row>
     <row r="144">
@@ -2664,7 +2664,7 @@
         <v>5</v>
       </c>
       <c r="D144">
-        <v>69.7964294180093</v>
+        <v>66.96560179304194</v>
       </c>
     </row>
     <row r="145">
@@ -2680,7 +2680,7 @@
         <v>6</v>
       </c>
       <c r="D145">
-        <v>75.60437889697127</v>
+        <v>73.44286776499123</v>
       </c>
     </row>
     <row r="146">
@@ -2696,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="D146">
-        <v>53.0520454127847</v>
+        <v>50.05259632421541</v>
       </c>
     </row>
     <row r="147">
@@ -2712,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="D147">
-        <v>58.99325739304629</v>
+        <v>56.70754563123086</v>
       </c>
     </row>
     <row r="148">
@@ -2728,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="D148">
-        <v>61.17586372982898</v>
+        <v>58.35102074694112</v>
       </c>
     </row>
     <row r="149">
@@ -2744,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="D149">
-        <v>66.2336720488222</v>
+        <v>63.82809850559875</v>
       </c>
     </row>
     <row r="150">
@@ -2760,7 +2760,7 @@
         <v>5</v>
       </c>
       <c r="D150">
-        <v>67.06383139036886</v>
+        <v>63.66831096099428</v>
       </c>
     </row>
     <row r="151">
@@ -2776,7 +2776,7 @@
         <v>6</v>
       </c>
       <c r="D151">
-        <v>69.61751686431757</v>
+        <v>65.80655825959256</v>
       </c>
     </row>
     <row r="152">
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="D152">
-        <v>58.41825353275907</v>
+        <v>53.66869367453739</v>
       </c>
     </row>
     <row r="153">
@@ -2808,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="D153">
-        <v>58.02873984953243</v>
+        <v>51.8826754302352</v>
       </c>
     </row>
     <row r="154">
@@ -2824,7 +2824,7 @@
         <v>3</v>
       </c>
       <c r="D154">
-        <v>56.27279929364034</v>
+        <v>48.27475468904574</v>
       </c>
     </row>
     <row r="155">
@@ -2840,7 +2840,7 @@
         <v>4</v>
       </c>
       <c r="D155">
-        <v>61.99311562847392</v>
+        <v>54.63517646882384</v>
       </c>
     </row>
     <row r="156">
@@ -2856,7 +2856,7 @@
         <v>5</v>
       </c>
       <c r="D156">
-        <v>64.07017312472324</v>
+        <v>56.13791979715628</v>
       </c>
     </row>
     <row r="157">
@@ -2872,7 +2872,7 @@
         <v>6</v>
       </c>
       <c r="D157">
-        <v>78.02304442516633</v>
+        <v>73.47508153108039</v>
       </c>
     </row>
     <row r="158">
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="D158">
-        <v>61.41281301828958</v>
+        <v>66.07637417270119</v>
       </c>
     </row>
     <row r="159">
@@ -2904,7 +2904,7 @@
         <v>2</v>
       </c>
       <c r="D159">
-        <v>60.4801389189</v>
+        <v>63.56614204018174</v>
       </c>
     </row>
     <row r="160">
@@ -2920,7 +2920,7 @@
         <v>3</v>
       </c>
       <c r="D160">
-        <v>66.70515626668531</v>
+        <v>70.5994985038955</v>
       </c>
     </row>
     <row r="161">
@@ -2936,7 +2936,7 @@
         <v>4</v>
       </c>
       <c r="D161">
-        <v>67.63255424523247</v>
+        <v>70.56936247529173</v>
       </c>
     </row>
     <row r="162">
@@ -2952,7 +2952,7 @@
         <v>5</v>
       </c>
       <c r="D162">
-        <v>71.24683340514231</v>
+        <v>74.12173468850483</v>
       </c>
     </row>
     <row r="163">
@@ -2968,7 +2968,7 @@
         <v>6</v>
       </c>
       <c r="D163">
-        <v>74.10976557543832</v>
+        <v>76.67231091556619</v>
       </c>
     </row>
     <row r="164">
@@ -2984,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="D164">
-        <v>54.32289443329449</v>
+        <v>54.34176963718104</v>
       </c>
     </row>
     <row r="165">
@@ -3000,7 +3000,7 @@
         <v>2</v>
       </c>
       <c r="D165">
-        <v>64.85946863768311</v>
+        <v>67.12386857636585</v>
       </c>
     </row>
     <row r="166">
@@ -3016,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="D166">
-        <v>63.54466186041671</v>
+        <v>64.10412620667732</v>
       </c>
     </row>
     <row r="167">
@@ -3032,7 +3032,7 @@
         <v>4</v>
       </c>
       <c r="D167">
-        <v>67.86448194495578</v>
+        <v>68.59721965272944</v>
       </c>
     </row>
     <row r="168">
@@ -3048,7 +3048,7 @@
         <v>5</v>
       </c>
       <c r="D168">
-        <v>72.03780852447031</v>
+        <v>72.89498842541546</v>
       </c>
     </row>
     <row r="169">
@@ -3064,7 +3064,7 @@
         <v>6</v>
       </c>
       <c r="D169">
-        <v>78.80417387112904</v>
+        <v>80.65014222096045</v>
       </c>
     </row>
     <row r="170">
@@ -3080,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="D170">
-        <v>51.97553463314176</v>
+        <v>46.90692305414919</v>
       </c>
     </row>
     <row r="171">
@@ -3096,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="D171">
-        <v>54.3462046748</v>
+        <v>48.80114977636016</v>
       </c>
     </row>
     <row r="172">
@@ -3112,7 +3112,7 @@
         <v>3</v>
       </c>
       <c r="D172">
-        <v>66.15081692318567</v>
+        <v>63.27396610754107</v>
       </c>
     </row>
     <row r="173">
@@ -3128,7 +3128,7 @@
         <v>4</v>
       </c>
       <c r="D173">
-        <v>63.60023647526025</v>
+        <v>58.60652551030717</v>
       </c>
     </row>
     <row r="174">
@@ -3144,7 +3144,7 @@
         <v>5</v>
       </c>
       <c r="D174">
-        <v>66.55452821615648</v>
+        <v>61.27891449816882</v>
       </c>
     </row>
     <row r="175">
@@ -3160,7 +3160,7 @@
         <v>6</v>
       </c>
       <c r="D175">
-        <v>68.81490676932621</v>
+        <v>63.02608590239514</v>
       </c>
     </row>
     <row r="176">
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="D176">
-        <v>54.45348267518646</v>
+        <v>58.18402663714837</v>
       </c>
     </row>
     <row r="177">
@@ -3192,7 +3192,7 @@
         <v>2</v>
       </c>
       <c r="D177">
-        <v>60.38570940424589</v>
+        <v>64.82699560922761</v>
       </c>
     </row>
     <row r="178">
@@ -3208,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="D178">
-        <v>67.76158729363944</v>
+        <v>73.39483279508566</v>
       </c>
     </row>
     <row r="179">
@@ -3224,7 +3224,7 @@
         <v>4</v>
       </c>
       <c r="D179">
-        <v>73.03717425892901</v>
+        <v>79.16228208213843</v>
       </c>
     </row>
     <row r="180">
@@ -3240,7 +3240,7 @@
         <v>5</v>
       </c>
       <c r="D180">
-        <v>75.63039490364662</v>
+        <v>81.35324294176192</v>
       </c>
     </row>
     <row r="181">
@@ -3256,7 +3256,7 @@
         <v>6</v>
       </c>
       <c r="D181">
-        <v>76.21665795085408</v>
+        <v>80.86826033803855</v>
       </c>
     </row>
     <row r="182">
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="D182">
-        <v>60.53217825510743</v>
+        <v>62.29778507839928</v>
       </c>
     </row>
     <row r="183">
@@ -3288,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="D183">
-        <v>62.73913905191341</v>
+        <v>63.7403994741406</v>
       </c>
     </row>
     <row r="184">
@@ -3304,7 +3304,7 @@
         <v>3</v>
       </c>
       <c r="D184">
-        <v>67.2012739582316</v>
+        <v>68.18991268256484</v>
       </c>
     </row>
     <row r="185">
@@ -3320,7 +3320,7 @@
         <v>4</v>
       </c>
       <c r="D185">
-        <v>76.50687993988439</v>
+        <v>79.09738732476856</v>
       </c>
     </row>
     <row r="186">
@@ -3336,7 +3336,7 @@
         <v>5</v>
       </c>
       <c r="D186">
-        <v>75.30615070714299</v>
+        <v>75.9964150144467</v>
       </c>
     </row>
     <row r="187">
@@ -3352,7 +3352,7 @@
         <v>6</v>
       </c>
       <c r="D187">
-        <v>88.71881033943102</v>
+        <v>92.37996119083074</v>
       </c>
     </row>
     <row r="188">
@@ -3368,7 +3368,7 @@
         <v>1</v>
       </c>
       <c r="D188">
-        <v>58.6388982521179</v>
+        <v>57.36829272618296</v>
       </c>
     </row>
     <row r="189">
@@ -3384,7 +3384,7 @@
         <v>2</v>
       </c>
       <c r="D189">
-        <v>64.05347351390311</v>
+        <v>63.08772640856323</v>
       </c>
     </row>
     <row r="190">
@@ -3400,7 +3400,7 @@
         <v>3</v>
       </c>
       <c r="D190">
-        <v>65.69427391979674</v>
+        <v>63.77546028308809</v>
       </c>
     </row>
     <row r="191">
@@ -3416,7 +3416,7 @@
         <v>4</v>
       </c>
       <c r="D191">
-        <v>70.68669096472566</v>
+        <v>68.93201634299331</v>
       </c>
     </row>
     <row r="192">
@@ -3432,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="D192">
-        <v>72.95880863709974</v>
+        <v>70.46150657282541</v>
       </c>
     </row>
     <row r="193">
@@ -3448,7 +3448,7 @@
         <v>6</v>
       </c>
       <c r="D193">
-        <v>80.86108086889728</v>
+        <v>79.49786954855547</v>
       </c>
     </row>
     <row r="194">
@@ -3464,7 +3464,7 @@
         <v>1</v>
       </c>
       <c r="D194">
-        <v>62.54719853686343</v>
+        <v>66.54668358596798</v>
       </c>
     </row>
     <row r="195">
@@ -3480,7 +3480,7 @@
         <v>2</v>
       </c>
       <c r="D195">
-        <v>66.76316435457419</v>
+        <v>70.66797134291565</v>
       </c>
     </row>
     <row r="196">
@@ -3496,7 +3496,7 @@
         <v>3</v>
       </c>
       <c r="D196">
-        <v>67.94564186092579</v>
+        <v>70.74460801805112</v>
       </c>
     </row>
     <row r="197">
@@ -3512,7 +3512,7 @@
         <v>4</v>
       </c>
       <c r="D197">
-        <v>72.42438540952804</v>
+        <v>75.21626608285412</v>
       </c>
     </row>
     <row r="198">
@@ -3528,7 +3528,7 @@
         <v>5</v>
       </c>
       <c r="D198">
-        <v>77.78365516706145</v>
+        <v>80.86195909289869</v>
       </c>
     </row>
     <row r="199">
@@ -3544,7 +3544,7 @@
         <v>6</v>
       </c>
       <c r="D199">
-        <v>88.27843333162909</v>
+        <v>93.35499664565553</v>
       </c>
     </row>
     <row r="200">
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="D200">
-        <v>57.84435611306885</v>
+        <v>60.21958644253527</v>
       </c>
     </row>
     <row r="201">
@@ -3576,7 +3576,7 @@
         <v>2</v>
       </c>
       <c r="D201">
-        <v>65.21911219192549</v>
+        <v>68.55259454767746</v>
       </c>
     </row>
     <row r="202">
@@ -3592,7 +3592,7 @@
         <v>3</v>
       </c>
       <c r="D202">
-        <v>75.96335244010287</v>
+        <v>81.37824821191396</v>
       </c>
     </row>
     <row r="203">
@@ -3608,7 +3608,7 @@
         <v>4</v>
       </c>
       <c r="D203">
-        <v>74.45334231907965</v>
+        <v>77.86490138388301</v>
       </c>
     </row>
     <row r="204">
@@ -3624,7 +3624,7 @@
         <v>5</v>
       </c>
       <c r="D204">
-        <v>75.1767448636019</v>
+        <v>77.32943810991267</v>
       </c>
     </row>
     <row r="205">
@@ -3640,7 +3640,7 @@
         <v>6</v>
       </c>
       <c r="D205">
-        <v>81.7619586692439</v>
+        <v>84.60972318410199</v>
       </c>
     </row>
     <row r="206">
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="D206">
-        <v>62.59954209998961</v>
+        <v>66.37132640544444</v>
       </c>
     </row>
     <row r="207">
@@ -3672,7 +3672,7 @@
         <v>2</v>
       </c>
       <c r="D207">
-        <v>64.51635354826566</v>
+        <v>67.42707500314583</v>
       </c>
     </row>
     <row r="208">
@@ -3688,7 +3688,7 @@
         <v>3</v>
       </c>
       <c r="D208">
-        <v>68.45753307262564</v>
+        <v>71.1819810356258</v>
       </c>
     </row>
     <row r="209">
@@ -3704,7 +3704,7 @@
         <v>4</v>
       </c>
       <c r="D209">
-        <v>73.6114104608896</v>
+        <v>76.55381755331109</v>
       </c>
     </row>
     <row r="210">
@@ -3720,7 +3720,7 @@
         <v>5</v>
       </c>
       <c r="D210">
-        <v>79.41465210469265</v>
+        <v>82.79147307838181</v>
       </c>
     </row>
     <row r="211">
@@ -3736,7 +3736,7 @@
         <v>6</v>
       </c>
       <c r="D211">
-        <v>88.43868847671246</v>
+        <v>93.32352157440823</v>
       </c>
     </row>
     <row r="212">
@@ -3752,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="D212">
-        <v>60.61158517178352</v>
+        <v>63.27758107604501</v>
       </c>
     </row>
     <row r="213">
@@ -3768,7 +3768,7 @@
         <v>2</v>
       </c>
       <c r="D213">
-        <v>68.61967899665474</v>
+        <v>72.45503950920661</v>
       </c>
     </row>
     <row r="214">
@@ -3784,7 +3784,7 @@
         <v>3</v>
       </c>
       <c r="D214">
-        <v>71.76954285515188</v>
+        <v>75.15485798720282</v>
       </c>
     </row>
     <row r="215">
@@ -3800,7 +3800,7 @@
         <v>4</v>
       </c>
       <c r="D215">
-        <v>74.03636082168177</v>
+        <v>76.67728194257599</v>
       </c>
     </row>
     <row r="216">
@@ -3816,7 +3816,7 @@
         <v>5</v>
       </c>
       <c r="D216">
-        <v>74.27857449952839</v>
+        <v>75.50023351303815</v>
       </c>
     </row>
     <row r="217">
@@ -3832,7 +3832,7 @@
         <v>6</v>
       </c>
       <c r="D217">
-        <v>81.81392855554263</v>
+        <v>84.04737225439047</v>
       </c>
     </row>
     <row r="218">
@@ -3848,7 +3848,7 @@
         <v>1</v>
       </c>
       <c r="D218">
-        <v>59.13822394765975</v>
+        <v>60.86402410867164</v>
       </c>
     </row>
     <row r="219">
@@ -3864,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="D219">
-        <v>65.24929860535975</v>
+        <v>67.51212365227164</v>
       </c>
     </row>
     <row r="220">
@@ -3880,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="D220">
-        <v>73.50843134007565</v>
+        <v>77.02430063189281</v>
       </c>
     </row>
     <row r="221">
@@ -3896,7 +3896,7 @@
         <v>4</v>
       </c>
       <c r="D221">
-        <v>80.98707222856846</v>
+        <v>85.49582181654991</v>
       </c>
     </row>
     <row r="222">
@@ -3912,7 +3912,7 @@
         <v>5</v>
       </c>
       <c r="D222">
-        <v>83.25057848402649</v>
+        <v>87.01383015716061</v>
       </c>
     </row>
     <row r="223">
@@ -3928,7 +3928,7 @@
         <v>6</v>
       </c>
       <c r="D223">
-        <v>82.70838241408835</v>
+        <v>84.79090206390975</v>
       </c>
     </row>
     <row r="224">
@@ -3944,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="D224">
-        <v>54.10659439217364</v>
+        <v>52.10242015430912</v>
       </c>
     </row>
     <row r="225">
@@ -3960,7 +3960,7 @@
         <v>2</v>
       </c>
       <c r="D225">
-        <v>62.70983698663132</v>
+        <v>62.07341028025269</v>
       </c>
     </row>
     <row r="226">
@@ -3976,7 +3976,7 @@
         <v>3</v>
       </c>
       <c r="D226">
-        <v>68.64379824806643</v>
+        <v>68.48535862883286</v>
       </c>
     </row>
     <row r="227">
@@ -3992,7 +3992,7 @@
         <v>4</v>
       </c>
       <c r="D227">
-        <v>75.41121559104886</v>
+        <v>76.00858175280942</v>
       </c>
     </row>
     <row r="228">
@@ -4008,7 +4008,7 @@
         <v>5</v>
       </c>
       <c r="D228">
-        <v>80.26376048429937</v>
+        <v>80.97864161047676</v>
       </c>
     </row>
     <row r="229">
@@ -4024,7 +4024,7 @@
         <v>6</v>
       </c>
       <c r="D229">
-        <v>83.92910486709594</v>
+        <v>84.36576745420554</v>
       </c>
     </row>
     <row r="230">
@@ -4040,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="D230">
-        <v>54.70225162312177</v>
+        <v>52.08312661836263</v>
       </c>
     </row>
     <row r="231">
@@ -4056,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="D231">
-        <v>65.93700380942023</v>
+        <v>65.56279620009391</v>
       </c>
     </row>
     <row r="232">
@@ -4072,7 +4072,7 @@
         <v>3</v>
       </c>
       <c r="D232">
-        <v>66.54840302323849</v>
+        <v>64.87799515185161</v>
       </c>
     </row>
     <row r="233">
@@ -4088,7 +4088,7 @@
         <v>4</v>
       </c>
       <c r="D233">
-        <v>72.91248277300393</v>
+        <v>71.86343481820552</v>
       </c>
     </row>
     <row r="234">
@@ -4104,7 +4104,7 @@
         <v>5</v>
       </c>
       <c r="D234">
-        <v>77.11172820404137</v>
+        <v>75.96242872625544</v>
       </c>
     </row>
     <row r="235">
@@ -4120,7 +4120,7 @@
         <v>6</v>
       </c>
       <c r="D235">
-        <v>82.67257496743167</v>
+        <v>81.87689107744252</v>
       </c>
     </row>
     <row r="236">
@@ -4136,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="D236">
-        <v>58.81308294645365</v>
+        <v>57.31587392523026</v>
       </c>
     </row>
     <row r="237">
@@ -4152,7 +4152,7 @@
         <v>2</v>
       </c>
       <c r="D237">
-        <v>58.23663270521825</v>
+        <v>55.04727360358305</v>
       </c>
     </row>
     <row r="238">
@@ -4168,7 +4168,7 @@
         <v>3</v>
       </c>
       <c r="D238">
-        <v>69.94854589229557</v>
+        <v>69.16315785301947</v>
       </c>
     </row>
     <row r="239">
@@ -4184,7 +4184,7 @@
         <v>4</v>
       </c>
       <c r="D239">
-        <v>73.39713770302427</v>
+        <v>72.26128026732439</v>
       </c>
     </row>
     <row r="240">
@@ -4200,7 +4200,7 @@
         <v>5</v>
       </c>
       <c r="D240">
-        <v>75.94210312214057</v>
+        <v>74.1545674928128</v>
       </c>
     </row>
     <row r="241">
@@ -4216,7 +4216,7 @@
         <v>6</v>
       </c>
       <c r="D241">
-        <v>81.59349153111528</v>
+        <v>80.18975203811242</v>
       </c>
     </row>
     <row r="242">
@@ -4232,7 +4232,7 @@
         <v>1</v>
       </c>
       <c r="D242">
-        <v>58.51270197826436</v>
+        <v>55.86791270795078</v>
       </c>
     </row>
     <row r="243">
@@ -4248,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="D243">
-        <v>63.27364444784197</v>
+        <v>60.71583600072093</v>
       </c>
     </row>
     <row r="244">
@@ -4264,7 +4264,7 @@
         <v>3</v>
       </c>
       <c r="D244">
-        <v>72.03312454009144</v>
+        <v>70.89514279038687</v>
       </c>
     </row>
     <row r="245">
@@ -4280,7 +4280,7 @@
         <v>4</v>
       </c>
       <c r="D245">
-        <v>70.95343490535855</v>
+        <v>67.95555661074303</v>
       </c>
     </row>
     <row r="246">
@@ -4296,7 +4296,7 @@
         <v>5</v>
       </c>
       <c r="D246">
-        <v>76.61478219381294</v>
+        <v>74.00401966201555</v>
       </c>
     </row>
     <row r="247">
@@ -4312,7 +4312,7 @@
         <v>6</v>
       </c>
       <c r="D247">
-        <v>84.11573766136625</v>
+        <v>82.5052936187533</v>
       </c>
     </row>
     <row r="248">
@@ -4328,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="D248">
-        <v>62.24670851409156</v>
+        <v>62.46922042539008</v>
       </c>
     </row>
     <row r="249">
@@ -4344,7 +4344,7 @@
         <v>2</v>
       </c>
       <c r="D249">
-        <v>67.01995477510187</v>
+        <v>67.33354877340383</v>
       </c>
     </row>
     <row r="250">
@@ -4360,7 +4360,7 @@
         <v>3</v>
       </c>
       <c r="D250">
-        <v>66.35176144078213</v>
+        <v>64.94262432764418</v>
       </c>
     </row>
     <row r="251">
@@ -4376,7 +4376,7 @@
         <v>4</v>
       </c>
       <c r="D251">
-        <v>78.59161363483929</v>
+        <v>79.76242725305373</v>
       </c>
     </row>
     <row r="252">
@@ -4392,7 +4392,7 @@
         <v>5</v>
       </c>
       <c r="D252">
-        <v>77.28426805675134</v>
+        <v>76.51929981560315</v>
       </c>
     </row>
     <row r="253">
@@ -4408,7 +4408,7 @@
         <v>6</v>
       </c>
       <c r="D253">
-        <v>87.18472097808139</v>
+        <v>88.21990371070986</v>
       </c>
     </row>
     <row r="254">
@@ -4424,7 +4424,7 @@
         <v>1</v>
       </c>
       <c r="D254">
-        <v>52.91649923877134</v>
+        <v>46.50401114646757</v>
       </c>
     </row>
     <row r="255">
@@ -4440,7 +4440,7 @@
         <v>2</v>
       </c>
       <c r="D255">
-        <v>61.53215805592619</v>
+        <v>56.49155623600736</v>
       </c>
     </row>
     <row r="256">
@@ -4456,7 +4456,7 @@
         <v>3</v>
       </c>
       <c r="D256">
-        <v>69.71895100977112</v>
+        <v>65.90728017446727</v>
       </c>
     </row>
     <row r="257">
@@ -4472,7 +4472,7 @@
         <v>4</v>
       </c>
       <c r="D257">
-        <v>68.32348073519509</v>
+        <v>62.54665314169922</v>
       </c>
     </row>
     <row r="258">
@@ -4488,7 +4488,7 @@
         <v>5</v>
       </c>
       <c r="D258">
-        <v>72.71114039221025</v>
+        <v>66.89686601771943</v>
       </c>
     </row>
     <row r="259">
@@ -4504,7 +4504,7 @@
         <v>6</v>
       </c>
       <c r="D259">
-        <v>76.65359118604279</v>
+        <v>70.65346707616283</v>
       </c>
     </row>
     <row r="260">
@@ -4520,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="D260">
-        <v>60.68037209266082</v>
+        <v>68.30368267467612</v>
       </c>
     </row>
     <row r="261">
@@ -4536,7 +4536,7 @@
         <v>2</v>
       </c>
       <c r="D261">
-        <v>67.02643333113583</v>
+        <v>75.26509765930948</v>
       </c>
     </row>
     <row r="262">
@@ -4552,7 +4552,7 @@
         <v>3</v>
       </c>
       <c r="D262">
-        <v>73.83144944955397</v>
+        <v>82.838452483867</v>
       </c>
     </row>
     <row r="263">
@@ -4568,7 +4568,7 @@
         <v>4</v>
       </c>
       <c r="D263">
-        <v>71.29528043691487</v>
+        <v>77.95689380034818</v>
       </c>
     </row>
     <row r="264">
@@ -4584,7 +4584,7 @@
         <v>5</v>
       </c>
       <c r="D264">
-        <v>82.47385323079389</v>
+        <v>91.36165752552024</v>
       </c>
     </row>
     <row r="265">
@@ -4600,7 +4600,7 @@
         <v>6</v>
       </c>
       <c r="D265">
-        <v>90.04793706992673</v>
+        <v>99.96043597769736</v>
       </c>
     </row>
     <row r="266">
@@ -4616,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="D266">
-        <v>68.02864605133129</v>
+        <v>74.89806806279168</v>
       </c>
     </row>
     <row r="267">
@@ -4632,7 +4632,7 @@
         <v>2</v>
       </c>
       <c r="D267">
-        <v>70.31945197321174</v>
+        <v>76.45247595863229</v>
       </c>
     </row>
     <row r="268">
@@ -4648,7 +4648,7 @@
         <v>3</v>
       </c>
       <c r="D268">
-        <v>73.18624828799786</v>
+        <v>78.77487104501378</v>
       </c>
     </row>
     <row r="269">
@@ -4664,7 +4664,7 @@
         <v>4</v>
       </c>
       <c r="D269">
-        <v>70.23573279926698</v>
+        <v>73.34085039337262</v>
       </c>
     </row>
     <row r="270">
@@ -4680,7 +4680,7 @@
         <v>5</v>
       </c>
       <c r="D270">
-        <v>78.11140387258963</v>
+        <v>82.34174515780282</v>
       </c>
     </row>
     <row r="271">
@@ -4696,7 +4696,7 @@
         <v>6</v>
       </c>
       <c r="D271">
-        <v>83.35978462686212</v>
+        <v>87.83958616349948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>